<commit_message>
generated all chimera cards, fix scripts
</commit_message>
<xml_diff>
--- a/Scripts/python/SourceTables/ChimeraEggs.xlsx
+++ b/Scripts/python/SourceTables/ChimeraEggs.xlsx
@@ -33,231 +33,153 @@
     <t>11400</t>
   </si>
   <si>
-    <t>Яйцо химеры: Сиба-ину</t>
-  </si>
-  <si>
     <t>Мощная духовная гончая Сиба-ину - Химера типа ФАТК. Преданность, выносливость, упорство и непоколебимая настойчивость лучше всего описывают это существо.</t>
   </si>
   <si>
     <t>11401</t>
   </si>
   <si>
-    <t>Яйцо химеры: Альпака</t>
-  </si>
-  <si>
     <t>Альпака - Химера типа Поддержки. Всегда остается непоколебимо преданной своему хозяину. Ее сердце, полное пылкой верности, всегда на страже своего владельца.</t>
   </si>
   <si>
     <t>11402</t>
   </si>
   <si>
-    <t>Яйцо химеры: Иллюзорник</t>
-  </si>
-  <si>
     <t>Иллюзорник - Химера MATK. Он создает сны и иллюзии, опьяняя мечтателей. Кто поддастся чарам станет его жертвой.</t>
   </si>
   <si>
     <t>11403</t>
   </si>
   <si>
-    <t>Яйцо химеры: Лисенок</t>
-  </si>
-  <si>
     <t>Милый Лисенок - Химера типа MATK. Все, кто хотел заполучить хвосты этого дивного существа, встретили трагическую гибель под его лапами.</t>
   </si>
   <si>
     <t>11404</t>
   </si>
   <si>
-    <t>Яйцо химеры: Медуза</t>
-  </si>
-  <si>
     <t>Солнечная Медуза является Химерой типа MATK. Ее щупальца, до краев наполненные ядом, служат ее самым грозным оружием, способным уничтожить любого врага.</t>
   </si>
   <si>
     <t>11405</t>
   </si>
   <si>
-    <t>Яйцо химеры: Журавль</t>
-  </si>
-  <si>
     <t>Благородный и утонченный Журавль - Химера типа Поддержки. Одно перо может закрыть солнце и луну, а крик может прогнать тысячи врагов.</t>
   </si>
   <si>
     <t>11406</t>
   </si>
   <si>
-    <t>Яйцо химеры: Златогребень</t>
-  </si>
-  <si>
     <t>Златогребень, Химера типа ФАТК, с момента своего рождения таит в себе единственную непоколебимую веру: сражаться, сражаться и еще раз сражаться!</t>
   </si>
   <si>
     <t>11407</t>
   </si>
   <si>
-    <t>Яйцо химеры: Лунный зверь</t>
-  </si>
-  <si>
     <t>Лунный зверь - это Химера типа ФАТК. Не обманывайтесь его внешним видом, его сила атаки ничуть не уступает другим Химерам.</t>
   </si>
   <si>
     <t>11408</t>
   </si>
   <si>
-    <t>Яйцо химеры: Русалка</t>
-  </si>
-  <si>
     <t>Русалка - Химера типа MATK, когда-то обитала на дне глубокого океана и обладала грозной силой.</t>
   </si>
   <si>
     <t>11409</t>
   </si>
   <si>
-    <t>Яйцо химеры: Тигрик</t>
-  </si>
-  <si>
     <t>Тигрик - Химера ФАТК. Именно из-за его необузданной натуры никто не может проследить его происхождение или расшифровать его неуловимую тактику.</t>
   </si>
   <si>
     <t>11410</t>
   </si>
   <si>
-    <t>Яйцо химеры: Барс</t>
-  </si>
-  <si>
     <t>Барс, некогда верховое животное горного демона, является Химерой поддержки. Мастерство Барса не имеет себе равных в этом мире.</t>
   </si>
   <si>
     <t>11411</t>
   </si>
   <si>
-    <t>Яйцо химеры: Цюнци</t>
-  </si>
-  <si>
     <t>Цюнци является Химерой поддержки с контролем одной цели. Когда Цюнци рычит, враги бросаются в рассыпную.</t>
   </si>
   <si>
     <t>11412</t>
   </si>
   <si>
-    <t>Яйцо химеры: Сорока</t>
-  </si>
-  <si>
     <t>Сорока парит в небесах среди редких звезд и стрекочет. Химера Защиты и Отражения. Выглядит безобидно, но ее силу в бою не стоит недооценивать.</t>
   </si>
   <si>
     <t>11413</t>
   </si>
   <si>
-    <t>Яйцо химеры: Дино</t>
-  </si>
-  <si>
     <t>Дино, существо типа ФАТК непревзойденной быстроты. Он не таит в себе никаких желаний, кроме одного - стать быстрее и сильнее!</t>
   </si>
   <si>
     <t>11414</t>
   </si>
   <si>
-    <t>Яйцо химеры: Сияющий мотылек</t>
-  </si>
-  <si>
     <t>Окутанный мистическим светом, Сияющий мотылек светится жизненной силой. Эта красочная Химера - целитель типа поддержки.</t>
   </si>
   <si>
     <t>11415</t>
   </si>
   <si>
-    <t>Яйцо химеры: Ледяной гигант</t>
-  </si>
-  <si>
     <t>Никто не знает его происхождения, известно лишь, что он полностью укутан снежным покровом. Ледяной гигант - это Химера типа ФАТК с контролем одной цели.</t>
   </si>
   <si>
     <t>11416</t>
   </si>
   <si>
-    <t>Яйцо химеры: Рыжий лис</t>
-  </si>
-  <si>
     <t>Рыжий лис. Стремится к безмятежной и свободной жизни. Химера Массового урона. Пламя рыжего лиса отпугивает тех, кто жаждет заполучить его мех.</t>
   </si>
   <si>
     <t>11417</t>
   </si>
   <si>
-    <t>Яйцо химеры: Трионикс</t>
-  </si>
-  <si>
     <t>Трионикс является Химерой поддержки, когда-то он процветал в глубинах Моря Реальности. Панцирь, покрывающий все его тело, подобен непроницаемому защитному щиту.</t>
   </si>
   <si>
     <t>11418</t>
   </si>
   <si>
-    <t>Яйцо химеры: Цилинь</t>
-  </si>
-  <si>
     <t>Цилинь - Химера урона в подземельях. Этот мифический фантомный зверь родился в хаосе объединения небесных и земных аур.</t>
   </si>
   <si>
     <t>11419</t>
   </si>
   <si>
-    <t>Яйцо химеры: Трехглавый феникс</t>
-  </si>
-  <si>
     <t>Трехглавый феникс - это Мифический зверь типа ФАТК с контролем одной цели. Одним взмахом крыльев он преодолевает тысячи миль сквозь облака.</t>
   </si>
   <si>
     <t>11420</t>
   </si>
   <si>
-    <t>Яйцо химеры: Цзяолун</t>
-  </si>
-  <si>
     <t>Цзяолун является Химерой типа поддержки. Эта Мифическая Химера одним звучным ревом может заставить отступить большинство других Химер или врагов.</t>
   </si>
   <si>
     <t>11421</t>
   </si>
   <si>
-    <t>Яйцо химеры: Сатх</t>
-  </si>
-  <si>
     <t>Сатх является ДД типа ФАТК по одной цели. Времена меняются, но этот Мифический зверь остается непревзойденным, его победа не вызывает сомнений.</t>
   </si>
   <si>
     <t>11422</t>
   </si>
   <si>
-    <t>Яйцо химеры: Феникс</t>
-  </si>
-  <si>
     <t>Феникс является Химерой типа поддержки. Своим звучным криком он может заставить небеса склониться, а пылающим пламенем испепелить врагов.</t>
   </si>
   <si>
     <t>11423</t>
   </si>
   <si>
-    <t>Яйцо химеры: Богиня Луны</t>
-  </si>
-  <si>
     <t>Богиня луны является химерой типа поддержки. С сердцем, полным сострадания, она дарит благословения всему живому.</t>
   </si>
   <si>
     <t>11424</t>
   </si>
   <si>
-    <t>Яйцо химеры: Тёмный Цзяолун</t>
-  </si>
-  <si>
     <t>11425</t>
   </si>
   <si>
-    <t>Яйцо химеры: Живоглот</t>
-  </si>
-  <si>
     <t>86206</t>
   </si>
   <si>
@@ -280,6 +202,84 @@
   </si>
   <si>
     <t>Даёт случайное яйцо Химеры: Богиня луны, Сатх, Трехглавый феникс, Цилинь. Призрачное яйцо продать нельзя.</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Сиба-ину</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Альпака</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Иллюзорник</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Лисенок</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Медуза</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Журавль</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Златогребень</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Лунный зверь</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Русалка</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Тигрик</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Барс</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Цюнци</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Сорока</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Дино</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Сияющий мотылек</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Ледяной гигант</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Рыжий лис</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Трионикс</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Цилинь</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Трехглавый феникс</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Цзяолун</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Сатх</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Феникс</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Богиня Луны</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Тёмный Цзяолун</t>
+  </si>
+  <si>
+    <t>Яйцо химеры Живоглот</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,6 +412,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,307 +747,307 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>